<commit_message>
Accidentally uploaded data dictionary without labels for a variable's margin of error. Uploading data dictionary with information on margins of error.
</commit_message>
<xml_diff>
--- a/Data Dictionary Stimulant Overdose Data.xlsx
+++ b/Data Dictionary Stimulant Overdose Data.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wfvdmei/Documents/Stimulant Overdose Data/Stimulant Overdose Dataset Creation/Stimulant Overdose Dataset Creation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39AED83-57D3-D245-95AF-B7257FD63E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E4DBAD-D6F9-2049-8AB6-144B17E7D23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8400" yWindow="500" windowWidth="27440" windowHeight="20720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blank Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Description of Fields" sheetId="2" r:id="rId2"/>
+    <sheet name="List of Variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="140">
   <si>
     <t>Element or value display name</t>
   </si>
@@ -36,167 +35,6 @@
   </si>
   <si>
     <t>Acceptable values</t>
-  </si>
-  <si>
-    <t>This can be used to manually create a data dictionary. Use one row for each data element, and do not leave rows, columns, or cells blank. Add rows and columns as necessary, and enter n/a if nothing applies. See below for an explanation of column headers.</t>
-  </si>
-  <si>
-    <t>Explanation of column headers:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Spreadsheet tab: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>If your spreadsheet has multiple tabs, identify the tab you are describing.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Element or value display name: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>What is the name used in your data file?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Description: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Write a brief definition, stated in the singular, that could stand alone from other element definitions.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Data type:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> For example, indicate varchar, integer, date, etc.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Character length:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> For example, the maximum length for Excel is 255, so indicate 255 or less.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Acceptable values: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>List all acceptable values, separated by pipes ( | ). This may be a field name or a range of values.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Required?: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Enter y/n to indicate whether this field is required.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Accepts null value?: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>This required to run calculations on your data. Indicate y/n if null value is allowable.</t>
-    </r>
-  </si>
-  <si>
-    <t>A note on null values: Null is the absence of a recorded value for a field. A null value differs from a value of zero in that zero may represent the measure of an attribute, while a null value indicates that no measurement has been taken.</t>
   </si>
   <si>
     <t>Variable Source</t>
@@ -480,12 +318,135 @@
   <si>
     <t>Greater than 0</t>
   </si>
+  <si>
+    <t>B15003_001_moe</t>
+  </si>
+  <si>
+    <t>B15003_003_moe</t>
+  </si>
+  <si>
+    <t>B15003_004_moe</t>
+  </si>
+  <si>
+    <t>B15003_005_moe</t>
+  </si>
+  <si>
+    <t>B15003_006_moe</t>
+  </si>
+  <si>
+    <t>B15003_007_moe</t>
+  </si>
+  <si>
+    <t>B15003_008_moe</t>
+  </si>
+  <si>
+    <t>B15003_009_moe</t>
+  </si>
+  <si>
+    <t>B15003_010_moe</t>
+  </si>
+  <si>
+    <t>B15003_011_moe</t>
+  </si>
+  <si>
+    <t>B15003_012_moe</t>
+  </si>
+  <si>
+    <t>B15003_013_moe</t>
+  </si>
+  <si>
+    <t>B15003_014_moe</t>
+  </si>
+  <si>
+    <t>B15003_015_moe</t>
+  </si>
+  <si>
+    <t>B15003_016_moe</t>
+  </si>
+  <si>
+    <t>B15003_017_moe</t>
+  </si>
+  <si>
+    <t>B15003_018_moe</t>
+  </si>
+  <si>
+    <t>B15003_019_moe</t>
+  </si>
+  <si>
+    <t>B15003_020_moe</t>
+  </si>
+  <si>
+    <t>B15003_021_moe</t>
+  </si>
+  <si>
+    <t>B15003_022_moe</t>
+  </si>
+  <si>
+    <t>B15003_023_moe</t>
+  </si>
+  <si>
+    <t>B15003_024_moe</t>
+  </si>
+  <si>
+    <t>B15003_025_moe</t>
+  </si>
+  <si>
+    <t>B17001_001_moe</t>
+  </si>
+  <si>
+    <t>B17001_002_moe</t>
+  </si>
+  <si>
+    <t>B25014_001_moe</t>
+  </si>
+  <si>
+    <t>B25014_002_moe</t>
+  </si>
+  <si>
+    <t>B25014_003_moe</t>
+  </si>
+  <si>
+    <t>B25014_004_moe</t>
+  </si>
+  <si>
+    <t>B25014_005_moe</t>
+  </si>
+  <si>
+    <t>B25014_006_moe</t>
+  </si>
+  <si>
+    <t>B25014_007_moe</t>
+  </si>
+  <si>
+    <t>B25014_008_moe</t>
+  </si>
+  <si>
+    <t>B25014_009_moe</t>
+  </si>
+  <si>
+    <t>B25014_010_moe</t>
+  </si>
+  <si>
+    <t>B25014_011_moe</t>
+  </si>
+  <si>
+    <t>B25014_012_moe</t>
+  </si>
+  <si>
+    <t>B25014_013_moe</t>
+  </si>
+  <si>
+    <t>B25064_001_moe</t>
+  </si>
+  <si>
+    <t>B25071_001_moe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -505,23 +466,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -583,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -601,20 +545,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,7 +871,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -948,13 +883,13 @@
   <sheetData>
     <row r="1" spans="1:25" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>90</v>
+      <c r="C1" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -989,23 +924,25 @@
     </row>
     <row r="2" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -1028,25 +965,25 @@
     </row>
     <row r="3" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -1069,23 +1006,25 @@
     </row>
     <row r="4" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -1108,23 +1047,25 @@
     </row>
     <row r="5" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1147,23 +1088,25 @@
     </row>
     <row r="6" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -1186,23 +1129,25 @@
     </row>
     <row r="7" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1225,23 +1170,25 @@
     </row>
     <row r="8" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1264,23 +1211,25 @@
     </row>
     <row r="9" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1303,23 +1252,25 @@
     </row>
     <row r="10" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1342,23 +1293,25 @@
     </row>
     <row r="11" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1381,23 +1334,25 @@
     </row>
     <row r="12" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1420,23 +1375,25 @@
     </row>
     <row r="13" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1459,23 +1416,25 @@
     </row>
     <row r="14" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1498,23 +1457,25 @@
     </row>
     <row r="15" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1537,23 +1498,25 @@
     </row>
     <row r="16" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1576,23 +1539,25 @@
     </row>
     <row r="17" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1615,23 +1580,25 @@
     </row>
     <row r="18" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1654,23 +1621,25 @@
     </row>
     <row r="19" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1693,23 +1662,25 @@
     </row>
     <row r="20" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1732,23 +1703,25 @@
     </row>
     <row r="21" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1771,23 +1744,25 @@
     </row>
     <row r="22" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1810,23 +1785,25 @@
     </row>
     <row r="23" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1849,23 +1826,25 @@
     </row>
     <row r="24" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1888,23 +1867,25 @@
     </row>
     <row r="25" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1927,23 +1908,25 @@
     </row>
     <row r="26" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1966,23 +1949,25 @@
     </row>
     <row r="27" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2005,23 +1990,25 @@
     </row>
     <row r="28" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2044,23 +2031,25 @@
     </row>
     <row r="29" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2083,23 +2072,25 @@
     </row>
     <row r="30" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2122,23 +2113,25 @@
     </row>
     <row r="31" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -2161,23 +2154,25 @@
     </row>
     <row r="32" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -2200,23 +2195,25 @@
     </row>
     <row r="33" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2239,23 +2236,25 @@
     </row>
     <row r="34" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>21</v>
+      <c r="C34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -2278,23 +2277,25 @@
     </row>
     <row r="35" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2317,23 +2318,25 @@
     </row>
     <row r="36" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>21</v>
+      <c r="C36" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2356,23 +2359,25 @@
     </row>
     <row r="37" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>21</v>
+      <c r="C37" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -2395,23 +2400,25 @@
     </row>
     <row r="38" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2434,23 +2441,25 @@
     </row>
     <row r="39" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
@@ -2473,23 +2482,25 @@
     </row>
     <row r="40" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2512,23 +2523,25 @@
     </row>
     <row r="41" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
@@ -2551,23 +2564,25 @@
     </row>
     <row r="42" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -2590,23 +2605,25 @@
     </row>
     <row r="43" spans="1:25" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11" t="s">
-        <v>106</v>
+        <v>6</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>20</v>
+        <v>96</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
@@ -28443,81 +28460,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="99" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>